<commit_message>
Execução diária para testar sem abrir o VsCode + 2 melhorias (to-dos) que vi a partir disso
</commit_message>
<xml_diff>
--- a/Bases/Lista de ações Tratada.xlsx
+++ b/Bases/Lista de ações Tratada.xlsx
@@ -19,7 +19,7 @@
     <t>Nome da Empresa</t>
   </si>
   <si>
-    <t>Volume no último dia útil (lido em 18/01/2025)</t>
+    <t>Volume no último dia útil (lido em 20/01/2025)</t>
   </si>
   <si>
     <t>Market Cap</t>
@@ -1839,7 +1839,7 @@
         <v>60743100</v>
       </c>
       <c r="D2">
-        <v>117830893568</v>
+        <v>117932556288</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1853,7 +1853,7 @@
         <v>58189500</v>
       </c>
       <c r="D3">
-        <v>16620328960</v>
+        <v>17139714048</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1867,7 +1867,7 @@
         <v>54658700</v>
       </c>
       <c r="D4">
-        <v>232602566656</v>
+        <v>230468206592</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1881,7 +1881,7 @@
         <v>51433600</v>
       </c>
       <c r="D5">
-        <v>174422409216</v>
+        <v>173636009984</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1895,7 +1895,7 @@
         <v>41057900</v>
       </c>
       <c r="D6">
-        <v>2305487616</v>
+        <v>2342375168</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1909,7 +1909,7 @@
         <v>39941100</v>
       </c>
       <c r="D7">
-        <v>512206798848</v>
+        <v>514409857024</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1923,7 +1923,7 @@
         <v>36310000</v>
       </c>
       <c r="D8">
-        <v>98601566208</v>
+        <v>100126883840</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1937,7 +1937,7 @@
         <v>30748300</v>
       </c>
       <c r="D9">
-        <v>54494822400</v>
+        <v>54916038656</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1951,7 +1951,7 @@
         <v>28519500</v>
       </c>
       <c r="D10">
-        <v>15275123712</v>
+        <v>14883931136</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1979,7 +1979,7 @@
         <v>23446400</v>
       </c>
       <c r="D12">
-        <v>4460505600</v>
+        <v>4541471744</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1993,7 +1993,7 @@
         <v>21683500</v>
       </c>
       <c r="D13">
-        <v>10781111296</v>
+        <v>10621980672</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2007,7 +2007,7 @@
         <v>20967900</v>
       </c>
       <c r="D14">
-        <v>26167351296</v>
+        <v>26224549888</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -2021,7 +2021,7 @@
         <v>20854200</v>
       </c>
       <c r="D15">
-        <v>296275181568</v>
+        <v>300396478464</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -2035,7 +2035,7 @@
         <v>18985500</v>
       </c>
       <c r="D16">
-        <v>21065242624</v>
+        <v>19929372672</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -2049,7 +2049,7 @@
         <v>18370400</v>
       </c>
       <c r="D17">
-        <v>12967830528</v>
+        <v>13115073536</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2063,7 +2063,7 @@
         <v>17814800</v>
       </c>
       <c r="D18">
-        <v>33730048000</v>
+        <v>34213746688</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -2077,7 +2077,7 @@
         <v>16929900</v>
       </c>
       <c r="D19">
-        <v>1541077248</v>
+        <v>1516726272</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -2091,7 +2091,7 @@
         <v>16881000</v>
       </c>
       <c r="D20">
-        <v>11916188672</v>
+        <v>12021641216</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -2119,7 +2119,7 @@
         <v>14778200</v>
       </c>
       <c r="D22">
-        <v>11762295808</v>
+        <v>11483788288</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -2133,7 +2133,7 @@
         <v>14463700</v>
       </c>
       <c r="D23">
-        <v>5443858944</v>
+        <v>5411836416</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -2147,7 +2147,7 @@
         <v>13941600</v>
       </c>
       <c r="D24">
-        <v>79408504832</v>
+        <v>80137650176</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -2161,7 +2161,7 @@
         <v>13271300</v>
       </c>
       <c r="D25">
-        <v>144696786944</v>
+        <v>145838374912</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -2175,7 +2175,7 @@
         <v>12833100</v>
       </c>
       <c r="D26">
-        <v>34414833664</v>
+        <v>34553524224</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -2189,7 +2189,7 @@
         <v>12831500</v>
       </c>
       <c r="D27">
-        <v>34721640448</v>
+        <v>35045679104</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -2203,7 +2203,7 @@
         <v>12546200</v>
       </c>
       <c r="D28">
-        <v>2368165632</v>
+        <v>2442688512</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -2217,7 +2217,7 @@
         <v>11699500</v>
       </c>
       <c r="D29">
-        <v>8107908096</v>
+        <v>8097658368</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -2231,7 +2231,7 @@
         <v>11169300</v>
       </c>
       <c r="D30">
-        <v>21387677696</v>
+        <v>21347473408</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -2245,7 +2245,7 @@
         <v>11149300</v>
       </c>
       <c r="D31">
-        <v>615655872</v>
+        <v>642095104</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -2259,7 +2259,7 @@
         <v>11027000</v>
       </c>
       <c r="D32">
-        <v>27812044800</v>
+        <v>27540443136</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -2273,7 +2273,7 @@
         <v>10647800</v>
       </c>
       <c r="D33">
-        <v>7847804416</v>
+        <v>7969161728</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -2287,7 +2287,7 @@
         <v>10545100</v>
       </c>
       <c r="D34">
-        <v>2966087936</v>
+        <v>3005485824</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -2301,7 +2301,7 @@
         <v>10152000</v>
       </c>
       <c r="D35">
-        <v>1691758080</v>
+        <v>1753175040</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -2315,7 +2315,7 @@
         <v>9730600</v>
       </c>
       <c r="D36">
-        <v>2953396480</v>
+        <v>2941629952</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -2329,7 +2329,7 @@
         <v>9197000</v>
       </c>
       <c r="D37">
-        <v>35817115648</v>
+        <v>36001611776</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -2343,7 +2343,7 @@
         <v>8985100</v>
       </c>
       <c r="D38">
-        <v>31591448576</v>
+        <v>31646971904</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -2357,7 +2357,7 @@
         <v>8708500</v>
       </c>
       <c r="D39">
-        <v>20916953088</v>
+        <v>20897638400</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -2371,7 +2371,7 @@
         <v>8658500</v>
       </c>
       <c r="D40">
-        <v>1323102720</v>
+        <v>1362305664</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -2385,7 +2385,7 @@
         <v>8454600</v>
       </c>
       <c r="D41">
-        <v>13608095744</v>
+        <v>13713585152</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -2399,7 +2399,7 @@
         <v>7855900</v>
       </c>
       <c r="D42">
-        <v>32076150784</v>
+        <v>32581951488</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -2413,7 +2413,7 @@
         <v>7731800</v>
       </c>
       <c r="D43">
-        <v>17201377280</v>
+        <v>17506316288</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -2427,7 +2427,7 @@
         <v>7648500</v>
       </c>
       <c r="D44">
-        <v>35849089024</v>
+        <v>35873292288</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -2441,7 +2441,7 @@
         <v>7539500</v>
       </c>
       <c r="D45">
-        <v>101255274496</v>
+        <v>101794406400</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -2455,7 +2455,7 @@
         <v>7500200</v>
       </c>
       <c r="D46">
-        <v>77179863040</v>
+        <v>76461105152</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -2469,7 +2469,7 @@
         <v>7256300</v>
       </c>
       <c r="D47">
-        <v>26167314432</v>
+        <v>26072961024</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -2483,7 +2483,7 @@
         <v>7182900</v>
       </c>
       <c r="D48">
-        <v>75083358208</v>
+        <v>76170240000</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -2497,7 +2497,7 @@
         <v>6877600</v>
       </c>
       <c r="D49">
-        <v>36345548800</v>
+        <v>36533866496</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -2511,7 +2511,7 @@
         <v>6836800</v>
       </c>
       <c r="D50">
-        <v>36922736640</v>
+        <v>38073528320</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -2525,7 +2525,7 @@
         <v>6704700</v>
       </c>
       <c r="D51">
-        <v>128619618304</v>
+        <v>130525970432</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -2539,7 +2539,7 @@
         <v>6693700</v>
       </c>
       <c r="D52">
-        <v>16781241344</v>
+        <v>17032662016</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -2553,7 +2553,7 @@
         <v>6521400</v>
       </c>
       <c r="D53">
-        <v>117830533120</v>
+        <v>118826287104</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -2567,7 +2567,7 @@
         <v>6260200</v>
       </c>
       <c r="D54">
-        <v>18976450560</v>
+        <v>19221737472</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -2581,7 +2581,7 @@
         <v>6218900</v>
       </c>
       <c r="D55">
-        <v>6549926912</v>
+        <v>6689208832</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -2595,7 +2595,7 @@
         <v>6170300</v>
       </c>
       <c r="D56">
-        <v>9761996800</v>
+        <v>9782145024</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -2609,7 +2609,7 @@
         <v>5627200</v>
       </c>
       <c r="D57">
-        <v>113549936</v>
+        <v>119808600</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -2623,7 +2623,7 @@
         <v>5328700</v>
       </c>
       <c r="D58">
-        <v>775153600</v>
+        <v>779651520</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -2637,7 +2637,7 @@
         <v>5264200</v>
       </c>
       <c r="D59">
-        <v>512208306176</v>
+        <v>516271505408</v>
       </c>
     </row>
     <row r="60" spans="1:4">
@@ -2651,7 +2651,7 @@
         <v>5192800</v>
       </c>
       <c r="D60">
-        <v>1423784320</v>
+        <v>1449096064</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -2679,7 +2679,7 @@
         <v>5126600</v>
       </c>
       <c r="D62">
-        <v>8129944576</v>
+        <v>8109044736</v>
       </c>
     </row>
     <row r="63" spans="1:4">
@@ -2693,7 +2693,7 @@
         <v>4948800</v>
       </c>
       <c r="D63">
-        <v>11572029440</v>
+        <v>11515085824</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -2707,7 +2707,7 @@
         <v>4930100</v>
       </c>
       <c r="D64">
-        <v>211415952</v>
+        <v>231174432</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -2721,7 +2721,7 @@
         <v>4849600</v>
       </c>
       <c r="D65">
-        <v>43989827584</v>
+        <v>44100018176</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -2735,7 +2735,7 @@
         <v>4675700</v>
       </c>
       <c r="D66">
-        <v>63566430208</v>
+        <v>64625872896</v>
       </c>
     </row>
     <row r="67" spans="1:4">
@@ -2749,7 +2749,7 @@
         <v>4456400</v>
       </c>
       <c r="D67">
-        <v>11301713920</v>
+        <v>11318915072</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -2763,7 +2763,7 @@
         <v>4282900</v>
       </c>
       <c r="D68">
-        <v>2433921536</v>
+        <v>2482660864</v>
       </c>
     </row>
     <row r="69" spans="1:4">
@@ -2777,7 +2777,7 @@
         <v>4222700</v>
       </c>
       <c r="D69">
-        <v>227272392704</v>
+        <v>229328207872</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -2791,7 +2791,7 @@
         <v>4169000</v>
       </c>
       <c r="D70">
-        <v>14073794560</v>
+        <v>14096276480</v>
       </c>
     </row>
     <row r="71" spans="1:4">
@@ -2805,7 +2805,7 @@
         <v>4084300</v>
       </c>
       <c r="D71">
-        <v>3234637568</v>
+        <v>3255506176</v>
       </c>
     </row>
     <row r="72" spans="1:4">
@@ -2819,7 +2819,7 @@
         <v>4079500</v>
       </c>
       <c r="D72">
-        <v>6421616640</v>
+        <v>6394667520</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -2833,7 +2833,7 @@
         <v>4011400</v>
       </c>
       <c r="D73">
-        <v>17193623552</v>
+        <v>17539657728</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -2847,7 +2847,7 @@
         <v>4002000</v>
       </c>
       <c r="D74">
-        <v>450118400</v>
+        <v>464184608</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -2861,7 +2861,7 @@
         <v>3894000</v>
       </c>
       <c r="D75">
-        <v>9339993088</v>
+        <v>9353489408</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -2875,7 +2875,7 @@
         <v>3893100</v>
       </c>
       <c r="D76">
-        <v>65565936</v>
+        <v>68774480</v>
       </c>
     </row>
     <row r="77" spans="1:4">
@@ -2889,7 +2889,7 @@
         <v>3803500</v>
       </c>
       <c r="D77">
-        <v>600035200</v>
+        <v>612667520</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -2903,7 +2903,7 @@
         <v>3778500</v>
       </c>
       <c r="D78">
-        <v>2837868032</v>
+        <v>2872266240</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -2917,7 +2917,7 @@
         <v>3753400</v>
       </c>
       <c r="D79">
-        <v>3333493760</v>
+        <v>3372558080</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -2931,7 +2931,7 @@
         <v>3608400</v>
       </c>
       <c r="D80">
-        <v>65565828</v>
+        <v>67362152</v>
       </c>
     </row>
     <row r="81" spans="1:4">
@@ -2945,7 +2945,7 @@
         <v>3594000</v>
       </c>
       <c r="D81">
-        <v>73435217920</v>
+        <v>73784631296</v>
       </c>
     </row>
     <row r="82" spans="1:4">
@@ -2973,7 +2973,7 @@
         <v>3376400</v>
       </c>
       <c r="D83">
-        <v>180826560</v>
+        <v>193383952</v>
       </c>
     </row>
     <row r="84" spans="1:4">
@@ -2987,7 +2987,7 @@
         <v>3215700</v>
       </c>
       <c r="D84">
-        <v>5013659136</v>
+        <v>5089296384</v>
       </c>
     </row>
     <row r="85" spans="1:4">
@@ -3001,7 +3001,7 @@
         <v>3162700</v>
       </c>
       <c r="D85">
-        <v>275702432</v>
+        <v>277603808</v>
       </c>
     </row>
     <row r="86" spans="1:4">
@@ -3015,7 +3015,7 @@
         <v>3104300</v>
       </c>
       <c r="D86">
-        <v>17285482496</v>
+        <v>17466245120</v>
       </c>
     </row>
     <row r="87" spans="1:4">
@@ -3029,7 +3029,7 @@
         <v>3050100</v>
       </c>
       <c r="D87">
-        <v>10032560128</v>
+        <v>10144955392</v>
       </c>
     </row>
     <row r="88" spans="1:4">
@@ -3043,7 +3043,7 @@
         <v>3019300</v>
       </c>
       <c r="D88">
-        <v>1469742336</v>
+        <v>1493130240</v>
       </c>
     </row>
     <row r="89" spans="1:4">
@@ -3057,7 +3057,7 @@
         <v>2997600</v>
       </c>
       <c r="D89">
-        <v>8235810816</v>
+        <v>8296479744</v>
       </c>
     </row>
     <row r="90" spans="1:4">
@@ -3071,7 +3071,7 @@
         <v>2973000</v>
       </c>
       <c r="D90">
-        <v>1299887744</v>
+        <v>1324885504</v>
       </c>
     </row>
     <row r="91" spans="1:4">
@@ -3085,7 +3085,7 @@
         <v>2897300</v>
       </c>
       <c r="D91">
-        <v>6280991232</v>
+        <v>6351747584</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -3099,7 +3099,7 @@
         <v>2888800</v>
       </c>
       <c r="D92">
-        <v>764684608</v>
+        <v>770266304</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -3113,7 +3113,7 @@
         <v>2883800</v>
       </c>
       <c r="D93">
-        <v>43439996928</v>
+        <v>43590000640</v>
       </c>
     </row>
     <row r="94" spans="1:4">
@@ -3127,7 +3127,7 @@
         <v>2872400</v>
       </c>
       <c r="D94">
-        <v>4273017600</v>
+        <v>4319667712</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -3141,7 +3141,7 @@
         <v>2736500</v>
       </c>
       <c r="D95">
-        <v>2588842752</v>
+        <v>2687677952</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -3155,7 +3155,7 @@
         <v>2647600</v>
       </c>
       <c r="D96">
-        <v>59299405824</v>
+        <v>59854434304</v>
       </c>
     </row>
     <row r="97" spans="1:4">
@@ -3169,7 +3169,7 @@
         <v>2618000</v>
       </c>
       <c r="D97">
-        <v>10525223936</v>
+        <v>10754415616</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -3183,7 +3183,7 @@
         <v>2550100</v>
       </c>
       <c r="D98">
-        <v>23596781568</v>
+        <v>23513354240</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -3197,7 +3197,7 @@
         <v>2547000</v>
       </c>
       <c r="D99">
-        <v>2486340608</v>
+        <v>2513513728</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -3211,7 +3211,7 @@
         <v>2515800</v>
       </c>
       <c r="D100">
-        <v>16522071040</v>
+        <v>16686118912</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -3239,7 +3239,7 @@
         <v>2474900</v>
       </c>
       <c r="D102">
-        <v>10107416576</v>
+        <v>10721679360</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -3253,7 +3253,7 @@
         <v>2458100</v>
       </c>
       <c r="D103">
-        <v>4769353728</v>
+        <v>4825938944</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -3267,7 +3267,7 @@
         <v>2273700</v>
       </c>
       <c r="D104">
-        <v>2243129856</v>
+        <v>2227922176</v>
       </c>
     </row>
     <row r="105" spans="1:4">
@@ -3281,7 +3281,7 @@
         <v>2166600</v>
       </c>
       <c r="D105">
-        <v>137883500544</v>
+        <v>138160816128</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -3295,7 +3295,7 @@
         <v>2026100</v>
       </c>
       <c r="D106">
-        <v>1596212224</v>
+        <v>1620087296</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -3309,7 +3309,7 @@
         <v>2022400</v>
       </c>
       <c r="D107">
-        <v>4513209856</v>
+        <v>4581378048</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -3323,7 +3323,7 @@
         <v>2017800</v>
       </c>
       <c r="D108">
-        <v>4143684352</v>
+        <v>4274710272</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -3337,7 +3337,7 @@
         <v>2012200</v>
       </c>
       <c r="D109">
-        <v>1935599872</v>
+        <v>1941343616</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -3365,7 +3365,7 @@
         <v>1999900</v>
       </c>
       <c r="D111">
-        <v>5658535936</v>
+        <v>5829567488</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -3379,7 +3379,7 @@
         <v>1928800</v>
       </c>
       <c r="D112">
-        <v>7787767296</v>
+        <v>7908042240</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -3393,7 +3393,7 @@
         <v>1928500</v>
       </c>
       <c r="D113">
-        <v>2460461312</v>
+        <v>2512811520</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -3407,7 +3407,7 @@
         <v>1827900</v>
       </c>
       <c r="D114">
-        <v>3698802432</v>
+        <v>3723710208</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -3421,7 +3421,7 @@
         <v>1823300</v>
       </c>
       <c r="D115">
-        <v>6260139520</v>
+        <v>6441832960</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -3435,7 +3435,7 @@
         <v>1816900</v>
       </c>
       <c r="D116">
-        <v>7594792448</v>
+        <v>7809521152</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -3449,7 +3449,7 @@
         <v>1771600</v>
       </c>
       <c r="D117">
-        <v>38300790784</v>
+        <v>38346878976</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -3463,7 +3463,7 @@
         <v>1725400</v>
       </c>
       <c r="D118">
-        <v>4378427392</v>
+        <v>4381887488</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -3477,7 +3477,7 @@
         <v>1699400</v>
       </c>
       <c r="D119">
-        <v>79869984768</v>
+        <v>79625994240</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -3491,7 +3491,7 @@
         <v>1676900</v>
       </c>
       <c r="D120">
-        <v>2615649792</v>
+        <v>2637286656</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -3505,7 +3505,7 @@
         <v>1587600</v>
       </c>
       <c r="D121">
-        <v>28720666624</v>
+        <v>28981762048</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -3519,7 +3519,7 @@
         <v>1584700</v>
       </c>
       <c r="D122">
-        <v>103160032</v>
+        <v>98499192</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -3533,7 +3533,7 @@
         <v>1525600</v>
       </c>
       <c r="D123">
-        <v>79408644096</v>
+        <v>79715794944</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -3547,7 +3547,7 @@
         <v>1510700</v>
       </c>
       <c r="D124">
-        <v>1763391488</v>
+        <v>1803152256</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -3561,7 +3561,7 @@
         <v>1507000</v>
       </c>
       <c r="D125">
-        <v>4697786368</v>
+        <v>4741040128</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -3575,7 +3575,7 @@
         <v>1480200</v>
       </c>
       <c r="D126">
-        <v>1143387520</v>
+        <v>1163411840</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -3589,7 +3589,7 @@
         <v>1459700</v>
       </c>
       <c r="D127">
-        <v>4891822592</v>
+        <v>4903546368</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -3603,7 +3603,7 @@
         <v>1396500</v>
       </c>
       <c r="D128">
-        <v>4300929536</v>
+        <v>4318574592</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -3617,7 +3617,7 @@
         <v>1302800</v>
       </c>
       <c r="D129">
-        <v>4125893120</v>
+        <v>4185688576</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -3631,7 +3631,7 @@
         <v>1299700</v>
       </c>
       <c r="D130">
-        <v>7937313280</v>
+        <v>7941720576</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -3645,7 +3645,7 @@
         <v>1287700</v>
       </c>
       <c r="D131">
-        <v>11244447744</v>
+        <v>11303013376</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -3659,7 +3659,7 @@
         <v>1280900</v>
       </c>
       <c r="D132">
-        <v>1651130624</v>
+        <v>1713437440</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -3673,7 +3673,7 @@
         <v>1168500</v>
       </c>
       <c r="D133">
-        <v>22225090560</v>
+        <v>22152300544</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -3687,7 +3687,7 @@
         <v>1157800</v>
       </c>
       <c r="D134">
-        <v>181790784</v>
+        <v>184444656</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -3701,7 +3701,7 @@
         <v>1079300</v>
       </c>
       <c r="D135">
-        <v>26808768512</v>
+        <v>26934335488</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -3743,7 +3743,7 @@
         <v>931000</v>
       </c>
       <c r="D138">
-        <v>1625361792</v>
+        <v>1653385216</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -3757,7 +3757,7 @@
         <v>891200</v>
       </c>
       <c r="D139">
-        <v>211415952</v>
+        <v>231174432</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -3771,7 +3771,7 @@
         <v>861400</v>
       </c>
       <c r="D140">
-        <v>7806884864</v>
+        <v>7964050432</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -3785,7 +3785,7 @@
         <v>848200</v>
       </c>
       <c r="D141">
-        <v>905183616</v>
+        <v>920269952</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -3799,7 +3799,7 @@
         <v>847700</v>
       </c>
       <c r="D142">
-        <v>1645262336</v>
+        <v>1664332928</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -3813,7 +3813,7 @@
         <v>846200</v>
       </c>
       <c r="D143">
-        <v>2920302336</v>
+        <v>2995182080</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -3827,7 +3827,7 @@
         <v>815100</v>
       </c>
       <c r="D144">
-        <v>8303784448</v>
+        <v>8478864896</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -3841,7 +3841,7 @@
         <v>808300</v>
       </c>
       <c r="D145">
-        <v>2026388096</v>
+        <v>1991940992</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -3855,7 +3855,7 @@
         <v>807000</v>
       </c>
       <c r="D146">
-        <v>5976598528</v>
+        <v>5943820288</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -3869,7 +3869,7 @@
         <v>779600</v>
       </c>
       <c r="D147">
-        <v>1236692352</v>
+        <v>1275449088</v>
       </c>
     </row>
     <row r="148" spans="1:4">
@@ -3883,7 +3883,7 @@
         <v>737600</v>
       </c>
       <c r="D148">
-        <v>751720960</v>
+        <v>755806400</v>
       </c>
     </row>
     <row r="149" spans="1:4">
@@ -3897,7 +3897,7 @@
         <v>696900</v>
       </c>
       <c r="D149">
-        <v>761693504</v>
+        <v>766272896</v>
       </c>
     </row>
     <row r="150" spans="1:4">
@@ -3911,7 +3911,7 @@
         <v>659900</v>
       </c>
       <c r="D150">
-        <v>93211744</v>
+        <v>91820520</v>
       </c>
     </row>
     <row r="151" spans="1:4">
@@ -3939,7 +3939,7 @@
         <v>634400</v>
       </c>
       <c r="D152">
-        <v>1102393600</v>
+        <v>1129953408</v>
       </c>
     </row>
     <row r="153" spans="1:4">
@@ -3967,7 +3967,7 @@
         <v>584600</v>
       </c>
       <c r="D154">
-        <v>14478970880</v>
+        <v>14383575040</v>
       </c>
     </row>
     <row r="155" spans="1:4">
@@ -3981,7 +3981,7 @@
         <v>579600</v>
       </c>
       <c r="D155">
-        <v>266738048</v>
+        <v>273711584</v>
       </c>
     </row>
     <row r="156" spans="1:4">
@@ -3995,7 +3995,7 @@
         <v>572600</v>
       </c>
       <c r="D156">
-        <v>296275345408</v>
+        <v>299518459904</v>
       </c>
     </row>
     <row r="157" spans="1:4">
@@ -4009,7 +4009,7 @@
         <v>568100</v>
       </c>
       <c r="D157">
-        <v>6503404032</v>
+        <v>6627438080</v>
       </c>
     </row>
     <row r="158" spans="1:4">
@@ -4023,7 +4023,7 @@
         <v>552400</v>
       </c>
       <c r="D158">
-        <v>1229216256</v>
+        <v>1244152192</v>
       </c>
     </row>
     <row r="159" spans="1:4">
@@ -4037,7 +4037,7 @@
         <v>524500</v>
       </c>
       <c r="D159">
-        <v>563463424</v>
+        <v>578657984</v>
       </c>
     </row>
     <row r="160" spans="1:4">
@@ -4051,7 +4051,7 @@
         <v>480100</v>
       </c>
       <c r="D160">
-        <v>6919831552</v>
+        <v>6929795072</v>
       </c>
     </row>
     <row r="161" spans="1:4">
@@ -4065,7 +4065,7 @@
         <v>477600</v>
       </c>
       <c r="D161">
-        <v>227569984</v>
+        <v>241921232</v>
       </c>
     </row>
     <row r="162" spans="1:4">
@@ -4079,7 +4079,7 @@
         <v>470800</v>
       </c>
       <c r="D162">
-        <v>1148310528</v>
+        <v>1155601408</v>
       </c>
     </row>
     <row r="163" spans="1:4">
@@ -4093,7 +4093,7 @@
         <v>462800</v>
       </c>
       <c r="D163">
-        <v>2361838592</v>
+        <v>2349342208</v>
       </c>
     </row>
     <row r="164" spans="1:4">
@@ -4107,7 +4107,7 @@
         <v>458300</v>
       </c>
       <c r="D164">
-        <v>4483273728</v>
+        <v>4480558592</v>
       </c>
     </row>
     <row r="165" spans="1:4">
@@ -4121,7 +4121,7 @@
         <v>453100</v>
       </c>
       <c r="D165">
-        <v>884285760</v>
+        <v>873092288</v>
       </c>
     </row>
     <row r="166" spans="1:4">
@@ -4135,7 +4135,7 @@
         <v>426300</v>
       </c>
       <c r="D166">
-        <v>1037171136</v>
+        <v>1029192960</v>
       </c>
     </row>
     <row r="167" spans="1:4">
@@ -4149,7 +4149,7 @@
         <v>407700</v>
       </c>
       <c r="D167">
-        <v>1944772864</v>
+        <v>1972004224</v>
       </c>
     </row>
     <row r="168" spans="1:4">
@@ -4163,7 +4163,7 @@
         <v>395300</v>
       </c>
       <c r="D168">
-        <v>1414942080</v>
+        <v>1422759552</v>
       </c>
     </row>
     <row r="169" spans="1:4">
@@ -4177,7 +4177,7 @@
         <v>394600</v>
       </c>
       <c r="D169">
-        <v>1992075904</v>
+        <v>2042508288</v>
       </c>
     </row>
     <row r="170" spans="1:4">
@@ -4191,7 +4191,7 @@
         <v>385600</v>
       </c>
       <c r="D170">
-        <v>2107296512</v>
+        <v>2157047296</v>
       </c>
     </row>
     <row r="171" spans="1:4">
@@ -4205,7 +4205,7 @@
         <v>377700</v>
       </c>
       <c r="D171">
-        <v>1387120768</v>
+        <v>1384105344</v>
       </c>
     </row>
     <row r="172" spans="1:4">
@@ -4219,7 +4219,7 @@
         <v>358100</v>
       </c>
       <c r="D172">
-        <v>1771059968</v>
+        <v>1802063232</v>
       </c>
     </row>
     <row r="173" spans="1:4">
@@ -4233,7 +4233,7 @@
         <v>342700</v>
       </c>
       <c r="D173">
-        <v>876535872</v>
+        <v>894497664</v>
       </c>
     </row>
     <row r="174" spans="1:4">
@@ -4247,7 +4247,7 @@
         <v>338100</v>
       </c>
       <c r="D174">
-        <v>1519310208</v>
+        <v>1527845504</v>
       </c>
     </row>
     <row r="175" spans="1:4">
@@ -4261,7 +4261,7 @@
         <v>336300</v>
       </c>
       <c r="D175">
-        <v>259753152</v>
+        <v>265462000</v>
       </c>
     </row>
     <row r="176" spans="1:4">
@@ -4275,7 +4275,7 @@
         <v>332400</v>
       </c>
       <c r="D176">
-        <v>320498240</v>
+        <v>327902496</v>
       </c>
     </row>
     <row r="177" spans="1:4">
@@ -4289,7 +4289,7 @@
         <v>329800</v>
       </c>
       <c r="D177">
-        <v>2966792704</v>
+        <v>2983168768</v>
       </c>
     </row>
     <row r="178" spans="1:4">
@@ -4317,7 +4317,7 @@
         <v>321200</v>
       </c>
       <c r="D179">
-        <v>1005237824</v>
+        <v>1009219008</v>
       </c>
     </row>
     <row r="180" spans="1:4">
@@ -4331,7 +4331,7 @@
         <v>294500</v>
       </c>
       <c r="D180">
-        <v>308703008</v>
+        <v>314877056</v>
       </c>
     </row>
     <row r="181" spans="1:4">
@@ -4345,7 +4345,7 @@
         <v>292800</v>
       </c>
       <c r="D181">
-        <v>1372103936</v>
+        <v>1376139520</v>
       </c>
     </row>
     <row r="182" spans="1:4">
@@ -4359,7 +4359,7 @@
         <v>288000</v>
       </c>
       <c r="D182">
-        <v>1200369920</v>
+        <v>1218022400</v>
       </c>
     </row>
     <row r="183" spans="1:4">
@@ -4373,7 +4373,7 @@
         <v>277300</v>
       </c>
       <c r="D183">
-        <v>3210401024</v>
+        <v>3239662592</v>
       </c>
     </row>
     <row r="184" spans="1:4">
@@ -4387,7 +4387,7 @@
         <v>268400</v>
       </c>
       <c r="D184">
-        <v>7271727104</v>
+        <v>7346693120</v>
       </c>
     </row>
     <row r="185" spans="1:4">
@@ -4401,7 +4401,7 @@
         <v>266000</v>
       </c>
       <c r="D185">
-        <v>3049274880</v>
+        <v>3055910912</v>
       </c>
     </row>
     <row r="186" spans="1:4">
@@ -4415,7 +4415,7 @@
         <v>244600</v>
       </c>
       <c r="D186">
-        <v>6230976000</v>
+        <v>6206540800</v>
       </c>
     </row>
     <row r="187" spans="1:4">
@@ -4443,7 +4443,7 @@
         <v>232300</v>
       </c>
       <c r="D188">
-        <v>52663376</v>
+        <v>53084680</v>
       </c>
     </row>
     <row r="189" spans="1:4">
@@ -4457,7 +4457,7 @@
         <v>227900</v>
       </c>
       <c r="D189">
-        <v>634468480</v>
+        <v>630263552</v>
       </c>
     </row>
     <row r="190" spans="1:4">
@@ -4471,7 +4471,7 @@
         <v>218100</v>
       </c>
       <c r="D190">
-        <v>3698859776</v>
+        <v>3666330112</v>
       </c>
     </row>
     <row r="191" spans="1:4">
@@ -4485,7 +4485,7 @@
         <v>216600</v>
       </c>
       <c r="D191">
-        <v>26808784896</v>
+        <v>26981742592</v>
       </c>
     </row>
     <row r="192" spans="1:4">
@@ -4499,7 +4499,7 @@
         <v>208600</v>
       </c>
       <c r="D192">
-        <v>2159393024</v>
+        <v>2171002624</v>
       </c>
     </row>
     <row r="193" spans="1:4">
@@ -4513,7 +4513,7 @@
         <v>207400</v>
       </c>
       <c r="D193">
-        <v>5575293952</v>
+        <v>5626027008</v>
       </c>
     </row>
     <row r="194" spans="1:4">
@@ -4527,7 +4527,7 @@
         <v>193400</v>
       </c>
       <c r="D194">
-        <v>7787750912</v>
+        <v>7940451840</v>
       </c>
     </row>
     <row r="195" spans="1:4">
@@ -4541,7 +4541,7 @@
         <v>187500</v>
       </c>
       <c r="D195">
-        <v>2234375680</v>
+        <v>2243341312</v>
       </c>
     </row>
     <row r="196" spans="1:4">
@@ -4555,7 +4555,7 @@
         <v>183000</v>
       </c>
       <c r="D196">
-        <v>1031891584</v>
+        <v>1036962304</v>
       </c>
     </row>
     <row r="197" spans="1:4">
@@ -4569,7 +4569,7 @@
         <v>174000</v>
       </c>
       <c r="D197">
-        <v>1165416320</v>
+        <v>1155193472</v>
       </c>
     </row>
     <row r="198" spans="1:4">
@@ -4583,7 +4583,7 @@
         <v>166100</v>
       </c>
       <c r="D198">
-        <v>11318201344</v>
+        <v>11307930624</v>
       </c>
     </row>
     <row r="199" spans="1:4">
@@ -4597,7 +4597,7 @@
         <v>164000</v>
       </c>
       <c r="D199">
-        <v>1178191744</v>
+        <v>1186277504</v>
       </c>
     </row>
     <row r="200" spans="1:4">
@@ -4611,7 +4611,7 @@
         <v>144100</v>
       </c>
       <c r="D200">
-        <v>1133974016</v>
+        <v>1151026176</v>
       </c>
     </row>
     <row r="201" spans="1:4">
@@ -4639,7 +4639,7 @@
         <v>135400</v>
       </c>
       <c r="D202">
-        <v>549384064</v>
+        <v>559652864</v>
       </c>
     </row>
     <row r="203" spans="1:4">
@@ -4653,7 +4653,7 @@
         <v>135000</v>
       </c>
       <c r="D203">
-        <v>8107865088</v>
+        <v>8216695296</v>
       </c>
     </row>
     <row r="204" spans="1:4">
@@ -4667,7 +4667,7 @@
         <v>130900</v>
       </c>
       <c r="D204">
-        <v>497684128</v>
+        <v>504733472</v>
       </c>
     </row>
     <row r="205" spans="1:4">
@@ -4681,7 +4681,7 @@
         <v>127300</v>
       </c>
       <c r="D205">
-        <v>33729961984</v>
+        <v>34033625088</v>
       </c>
     </row>
     <row r="206" spans="1:4">
@@ -4695,7 +4695,7 @@
         <v>125400</v>
       </c>
       <c r="D206">
-        <v>6421614080</v>
+        <v>6364351488</v>
       </c>
     </row>
     <row r="207" spans="1:4">
@@ -4709,7 +4709,7 @@
         <v>116400</v>
       </c>
       <c r="D207">
-        <v>816175360</v>
+        <v>814311936</v>
       </c>
     </row>
     <row r="208" spans="1:4">
@@ -4723,7 +4723,7 @@
         <v>113200</v>
       </c>
       <c r="D208">
-        <v>4088953856</v>
+        <v>4072235520</v>
       </c>
     </row>
     <row r="209" spans="1:4">
@@ -4737,7 +4737,7 @@
         <v>105200</v>
       </c>
       <c r="D209">
-        <v>1630947840</v>
+        <v>1634429184</v>
       </c>
     </row>
     <row r="210" spans="1:4">
@@ -4751,7 +4751,7 @@
         <v>100400</v>
       </c>
       <c r="D210">
-        <v>11318232064</v>
+        <v>11287081984</v>
       </c>
     </row>
     <row r="211" spans="1:4">
@@ -4779,7 +4779,7 @@
         <v>91300</v>
       </c>
       <c r="D212">
-        <v>227030448</v>
+        <v>229525280</v>
       </c>
     </row>
     <row r="213" spans="1:4">
@@ -4793,7 +4793,7 @@
         <v>88000</v>
       </c>
       <c r="D213">
-        <v>843375680</v>
+        <v>838029376</v>
       </c>
     </row>
     <row r="214" spans="1:4">
@@ -4807,7 +4807,7 @@
         <v>85100</v>
       </c>
       <c r="D214">
-        <v>305134880</v>
+        <v>307665024</v>
       </c>
     </row>
     <row r="215" spans="1:4">
@@ -4821,7 +4821,7 @@
         <v>80900</v>
       </c>
       <c r="D215">
-        <v>5118996992</v>
+        <v>5204463616</v>
       </c>
     </row>
     <row r="216" spans="1:4">
@@ -4835,7 +4835,7 @@
         <v>79900</v>
       </c>
       <c r="D216">
-        <v>776127616</v>
+        <v>781032064</v>
       </c>
     </row>
     <row r="217" spans="1:4">
@@ -4849,7 +4849,7 @@
         <v>78800</v>
       </c>
       <c r="D217">
-        <v>98601467904</v>
+        <v>99782959104</v>
       </c>
     </row>
     <row r="218" spans="1:4">
@@ -4863,7 +4863,7 @@
         <v>78100</v>
       </c>
       <c r="D218">
-        <v>92722085888</v>
+        <v>93148069888</v>
       </c>
     </row>
     <row r="219" spans="1:4">
@@ -4877,7 +4877,7 @@
         <v>77000</v>
       </c>
       <c r="D219">
-        <v>1166937216</v>
+        <v>1204989440</v>
       </c>
     </row>
     <row r="220" spans="1:4">
@@ -4891,7 +4891,7 @@
         <v>71700</v>
       </c>
       <c r="D220">
-        <v>953176256</v>
+        <v>984695232</v>
       </c>
     </row>
     <row r="221" spans="1:4">
@@ -4905,7 +4905,7 @@
         <v>71100</v>
       </c>
       <c r="D221">
-        <v>586454400</v>
+        <v>566556800</v>
       </c>
     </row>
     <row r="222" spans="1:4">
@@ -4919,7 +4919,7 @@
         <v>68200</v>
       </c>
       <c r="D222">
-        <v>308867008</v>
+        <v>312566016</v>
       </c>
     </row>
     <row r="223" spans="1:4">
@@ -4933,7 +4933,7 @@
         <v>67400</v>
       </c>
       <c r="D223">
-        <v>568038272</v>
+        <v>559431552</v>
       </c>
     </row>
     <row r="224" spans="1:4">
@@ -4947,7 +4947,7 @@
         <v>65600</v>
       </c>
       <c r="D224">
-        <v>4993673728</v>
+        <v>4922335744</v>
       </c>
     </row>
     <row r="225" spans="1:4">
@@ -4961,7 +4961,7 @@
         <v>65600</v>
       </c>
       <c r="D225">
-        <v>4993673728</v>
+        <v>4922335744</v>
       </c>
     </row>
     <row r="226" spans="1:4">
@@ -4975,7 +4975,7 @@
         <v>61500</v>
       </c>
       <c r="D226">
-        <v>227030448</v>
+        <v>232020128</v>
       </c>
     </row>
     <row r="227" spans="1:4">
@@ -4989,7 +4989,7 @@
         <v>60600</v>
       </c>
       <c r="D227">
-        <v>235956480</v>
+        <v>239643312</v>
       </c>
     </row>
     <row r="228" spans="1:4">
@@ -5003,7 +5003,7 @@
         <v>60400</v>
       </c>
       <c r="D228">
-        <v>92722110464</v>
+        <v>92329885696</v>
       </c>
     </row>
     <row r="229" spans="1:4">
@@ -5017,7 +5017,7 @@
         <v>59600</v>
       </c>
       <c r="D229">
-        <v>988200448</v>
+        <v>974724992</v>
       </c>
     </row>
     <row r="230" spans="1:4">
@@ -5031,7 +5031,7 @@
         <v>58900</v>
       </c>
       <c r="D230">
-        <v>301600864</v>
+        <v>306986592</v>
       </c>
     </row>
     <row r="231" spans="1:4">
@@ -5045,7 +5045,7 @@
         <v>57800</v>
       </c>
       <c r="D231">
-        <v>9761969152</v>
+        <v>9712010240</v>
       </c>
     </row>
     <row r="232" spans="1:4">
@@ -5059,7 +5059,7 @@
         <v>57800</v>
       </c>
       <c r="D232">
-        <v>2588844032</v>
+        <v>2637427968</v>
       </c>
     </row>
     <row r="233" spans="1:4">
@@ -5073,7 +5073,7 @@
         <v>54000</v>
       </c>
       <c r="D233">
-        <v>1357032832</v>
+        <v>1358561024</v>
       </c>
     </row>
     <row r="234" spans="1:4">
@@ -5087,7 +5087,7 @@
         <v>48500</v>
       </c>
       <c r="D234">
-        <v>243276320</v>
+        <v>244853472</v>
       </c>
     </row>
     <row r="235" spans="1:4">
@@ -5101,7 +5101,7 @@
         <v>48200</v>
       </c>
       <c r="D235">
-        <v>145961440</v>
+        <v>147865296</v>
       </c>
     </row>
     <row r="236" spans="1:4">
@@ -5115,7 +5115,7 @@
         <v>45500</v>
       </c>
       <c r="D236">
-        <v>20732991488</v>
+        <v>20577869824</v>
       </c>
     </row>
     <row r="237" spans="1:4">
@@ -5129,7 +5129,7 @@
         <v>42800</v>
       </c>
       <c r="D237">
-        <v>186599760</v>
+        <v>189055008</v>
       </c>
     </row>
     <row r="238" spans="1:4">
@@ -5143,7 +5143,7 @@
         <v>40500</v>
       </c>
       <c r="D238">
-        <v>122920704</v>
+        <v>120277248</v>
       </c>
     </row>
     <row r="239" spans="1:4">
@@ -5157,7 +5157,7 @@
         <v>40000</v>
       </c>
       <c r="D239">
-        <v>108956416</v>
+        <v>107484032</v>
       </c>
     </row>
     <row r="240" spans="1:4">
@@ -5171,7 +5171,7 @@
         <v>39200</v>
       </c>
       <c r="D240">
-        <v>1925486848</v>
+        <v>1923875456</v>
       </c>
     </row>
     <row r="241" spans="1:4">
@@ -5185,7 +5185,7 @@
         <v>37900</v>
       </c>
       <c r="D241">
-        <v>672053056</v>
+        <v>670814656</v>
       </c>
     </row>
     <row r="242" spans="1:4">
@@ -5199,7 +5199,7 @@
         <v>37600</v>
       </c>
       <c r="D242">
-        <v>469821792</v>
+        <v>458934656</v>
       </c>
     </row>
     <row r="243" spans="1:4">
@@ -5213,7 +5213,7 @@
         <v>36400</v>
       </c>
       <c r="D243">
-        <v>182099952</v>
+        <v>180589120</v>
       </c>
     </row>
     <row r="244" spans="1:4">
@@ -5241,7 +5241,7 @@
         <v>32100</v>
       </c>
       <c r="D245">
-        <v>649007104</v>
+        <v>645244736</v>
       </c>
     </row>
     <row r="246" spans="1:4">
@@ -5255,7 +5255,7 @@
         <v>28700</v>
       </c>
       <c r="D246">
-        <v>34414903296</v>
+        <v>34566221824</v>
       </c>
     </row>
     <row r="247" spans="1:4">
@@ -5269,7 +5269,7 @@
         <v>28700</v>
       </c>
       <c r="D247">
-        <v>56499012</v>
+        <v>56894116</v>
       </c>
     </row>
     <row r="248" spans="1:4">
@@ -5283,7 +5283,7 @@
         <v>26300</v>
       </c>
       <c r="D248">
-        <v>2132368896</v>
+        <v>2126003584</v>
       </c>
     </row>
     <row r="249" spans="1:4">
@@ -5311,7 +5311,7 @@
         <v>23700</v>
       </c>
       <c r="D250">
-        <v>1327658112</v>
+        <v>1311302784</v>
       </c>
     </row>
     <row r="251" spans="1:4">
@@ -5325,7 +5325,7 @@
         <v>20700</v>
       </c>
       <c r="D251">
-        <v>192900256</v>
+        <v>186808672</v>
       </c>
     </row>
   </sheetData>

</xml_diff>